<commit_message>
Member API RestAPI 적용
</commit_message>
<xml_diff>
--- a/설계.xlsx
+++ b/설계.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeojin\Software Projects\Spring-Boot-Projects\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B408D267-CF5B-4922-9D3B-DD354F81B208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C155CF-5891-4D6D-A331-CDF76B63CA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D6293FF8-81F7-4313-A4CE-927893CD5DFF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D6293FF8-81F7-4313-A4CE-927893CD5DFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="게시판 조회" sheetId="1" r:id="rId2"/>
-    <sheet name="게시글 등록" sheetId="2" r:id="rId3"/>
-    <sheet name="댓글" sheetId="5" r:id="rId4"/>
-    <sheet name="ERD" sheetId="4" r:id="rId5"/>
+    <sheet name="개발 내용" sheetId="6" r:id="rId1"/>
+    <sheet name="API Sheet" sheetId="7" r:id="rId2"/>
+    <sheet name="게시판 조회" sheetId="1" r:id="rId3"/>
+    <sheet name="게시글 등록" sheetId="2" r:id="rId4"/>
+    <sheet name="댓글" sheetId="5" r:id="rId5"/>
+    <sheet name="ERD" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
   <si>
     <t>게시판 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,7 +347,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ㄴ</t>
+    <t>URI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API 카테고리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTTP URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTTP Method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mandatory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response Parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>localhost:8080/member/login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -354,7 +463,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,8 +527,17 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +568,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -767,7 +903,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -870,6 +1006,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,6 +1065,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1384,73 +1541,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9BAEE9-CF58-4BD4-B955-7A522030867E}">
-  <dimension ref="B2:F34"/>
+  <dimension ref="B2:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>75</v>
       </c>
@@ -1462,6 +1616,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E59DFC-F78A-4EF3-B6E8-34D71937F871}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.58203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.58203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="10.08203125" customWidth="1"/>
+    <col min="7" max="7" width="9.4140625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B4" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C5" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B7" s="55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B9" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="34">
+        <v>1234</v>
+      </c>
+      <c r="H11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B12" s="55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B14" s="58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD08B8B3-38DF-4270-87E0-DC9D2278E231}">
   <dimension ref="C3:O24"/>
   <sheetViews>
@@ -1469,18 +1767,18 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="22.625" customWidth="1"/>
-    <col min="15" max="15" width="11.875" customWidth="1"/>
+    <col min="14" max="14" width="22.58203125" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1488,13 +1786,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1514,7 +1812,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.45">
       <c r="M7">
         <v>1</v>
       </c>
@@ -1525,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
@@ -1551,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C9" s="1">
         <v>1</v>
       </c>
@@ -1577,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C10" s="1">
         <v>2</v>
       </c>
@@ -1594,7 +1892,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C11" s="1">
         <v>3</v>
       </c>
@@ -1611,7 +1909,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C12" s="1">
         <v>4</v>
       </c>
@@ -1628,7 +1926,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C13" s="1">
         <v>5</v>
       </c>
@@ -1645,7 +1943,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C14" s="1">
         <v>6</v>
       </c>
@@ -1662,46 +1960,46 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C18"/>
       <c r="D18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C20"/>
       <c r="D20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C21"/>
       <c r="E21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C22"/>
       <c r="E22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>66</v>
       </c>
@@ -1713,7 +2011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883D50C-33B2-480D-952C-22F3ACA7BFCE}">
   <dimension ref="C3:J37"/>
   <sheetViews>
@@ -1721,18 +2019,18 @@
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="4" max="4" width="3.75" customWidth="1"/>
-    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +2041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -1754,7 +2052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>5</v>
       </c>
@@ -1765,19 +2063,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="J12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>22</v>
       </c>
@@ -1789,79 +2087,79 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.45">
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.45">
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>24</v>
       </c>
@@ -1875,7 +2173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6385002-3272-4EDB-969E-4F1CD27BE425}">
   <dimension ref="B3:M47"/>
   <sheetViews>
@@ -1883,42 +2181,42 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="1.875" customWidth="1"/>
-    <col min="5" max="5" width="1.625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="1.83203125" customWidth="1"/>
+    <col min="5" max="5" width="1.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B3" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="39" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B7" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -1927,18 +2225,18 @@
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="41" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -1947,12 +2245,12 @@
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -1961,12 +2259,12 @@
       <c r="G13" s="18"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1975,7 +2273,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -1984,7 +2282,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1993,7 +2291,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2002,7 +2300,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2011,7 +2309,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -2020,7 +2318,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B23" s="29" t="s">
         <v>40</v>
       </c>
@@ -2031,12 +2329,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="37" t="s">
+    <row r="25" spans="2:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B26" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="38"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
@@ -2049,28 +2347,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="44" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B27" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="48"/>
       <c r="M27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="50" t="s">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B28" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="51"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
@@ -2083,25 +2381,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="44" t="s">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B29" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="46"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="50" t="s">
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="48"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B30" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="51"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -2114,28 +2412,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="44" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B31" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="46"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="48"/>
       <c r="M31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="50" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B32" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="51"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -2148,28 +2446,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="44" t="s">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B33" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="48"/>
       <c r="M33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="50" t="s">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B34" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="51"/>
+      <c r="C34" s="53"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -2182,26 +2480,26 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="47" t="s">
+    <row r="35" spans="2:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="49"/>
-    </row>
-    <row r="36" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="37" t="s">
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="51"/>
+    </row>
+    <row r="36" spans="2:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B37" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="38"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
@@ -2211,7 +2509,7 @@
       <c r="J37" s="21"/>
       <c r="K37" s="22"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B38" s="24" t="s">
         <v>44</v>
       </c>
@@ -2225,7 +2523,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="25"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B39" s="26"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -2237,7 +2535,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="25"/>
     </row>
-    <row r="40" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B40" s="27"/>
       <c r="C40" s="28"/>
       <c r="D40" s="28"/>
@@ -2251,27 +2549,27 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.45">
       <c r="M43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.45">
       <c r="M44" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.45">
       <c r="M45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.45">
       <c r="M46" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
       <c r="M47" t="s">
         <v>56</v>
       </c>
@@ -2300,7 +2598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4664C19-9071-4B69-80D3-697E1485FAA0}">
   <dimension ref="K4:K5"/>
   <sheetViews>
@@ -2308,14 +2606,14 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="4" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K5" t="s">
         <v>35</v>
       </c>

</xml_diff>